<commit_message>
update after first task
</commit_message>
<xml_diff>
--- a/Linear Programming/gen_stations.xlsx
+++ b/Linear Programming/gen_stations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abayomi\Desktop\Linear Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abayomi\Desktop\Basic-Energy-System-Optimization\Linear Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E77DF94-F28F-4A30-9E3B-526500E0D480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226E7157-7A3E-4E70-8B53-DDE9FC7231C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CB57A7E7-BB22-474B-B142-9B359C5189D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Stations</t>
   </si>
@@ -68,12 +68,6 @@
     <t>Sapele NIPP</t>
   </si>
   <si>
-    <t>Geregu NIPP</t>
-  </si>
-  <si>
-    <t>Geregu Gas</t>
-  </si>
-  <si>
     <t>Omotosho (Gas)</t>
   </si>
   <si>
@@ -102,6 +96,21 @@
   </si>
   <si>
     <t>Afam VI (Gas)</t>
+  </si>
+  <si>
+    <t>Geregu NIPP (Gas)</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Fuel type</t>
+  </si>
+  <si>
+    <t>Geregu II (Gas)</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -299,26 +308,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2ED293-C79D-48EB-B8A9-9E6CE0BD60A4}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +657,7 @@
     <col min="3" max="3" width="36.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -655,31 +665,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="16">
         <v>760</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="16">
         <v>327</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-    </row>
-    <row r="4" spans="1:3" hidden="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" hidden="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="15"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -689,8 +711,11 @@
       <c r="C5" s="3">
         <v>351</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -700,8 +725,11 @@
       <c r="C6" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -711,9 +739,12 @@
       <c r="C7" s="3">
         <v>1100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17" t="s">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="9">
@@ -722,8 +753,11 @@
       <c r="C8" s="9">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -733,8 +767,11 @@
       <c r="C9" s="9">
         <v>604</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -744,10 +781,13 @@
       <c r="C10" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3">
         <v>650</v>
@@ -755,8 +795,11 @@
       <c r="C11" s="3">
         <v>576</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -766,10 +809,13 @@
       <c r="C12" s="3">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3">
         <v>450</v>
@@ -777,10 +823,13 @@
       <c r="C13" s="3">
         <v>435</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3">
         <v>450</v>
@@ -788,10 +837,13 @@
       <c r="C14" s="3">
         <v>435</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>335</v>
@@ -799,10 +851,13 @@
       <c r="C15" s="3">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
         <v>500</v>
@@ -810,10 +865,13 @@
       <c r="C16" s="3">
         <v>360</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="9">
         <v>500</v>
@@ -821,10 +879,13 @@
       <c r="C17" s="9">
         <v>360</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="3">
         <v>335</v>
@@ -832,10 +893,13 @@
       <c r="C18" s="3">
         <v>240</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3">
         <v>750</v>
@@ -843,10 +907,13 @@
       <c r="C19" s="3">
         <v>300</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3">
         <v>461</v>
@@ -854,10 +921,13 @@
       <c r="C20" s="3">
         <v>450</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="9">
         <v>480</v>
@@ -865,10 +935,13 @@
       <c r="C21" s="9">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22" s="5">
         <v>500</v>
@@ -876,8 +949,11 @@
       <c r="C22" s="5">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A4"/>

</xml_diff>